<commit_message>
Unidades mudando alguns nomes
</commit_message>
<xml_diff>
--- a/Acervo em 31-05-2020 às 22-22-52.xlsx
+++ b/Acervo em 31-05-2020 às 22-22-52.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fe9feb4c34dc3191/Área de Trabalho/Estudo Competências/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mecao\OneDrive\Documentos\PRODUTIVIDADE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5392E7E-3C1D-4336-915B-7AE1F998C47C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B83B79-85D7-4304-A7A6-F92BB4010D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="600" windowWidth="19200" windowHeight="15600" xr2:uid="{0104159D-1B62-4070-BC97-643D266733BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0104159D-1B62-4070-BC97-643D266733BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -362,9 +362,6 @@
     <t>NATAL - 16ª VARA CRIMINAL</t>
   </si>
   <si>
-    <t>NATAL - 17ª VARA CRIMINAL</t>
-  </si>
-  <si>
     <t>NATAL - 1ª VARA DA INFÂNCIA E JUVENTUDE</t>
   </si>
   <si>
@@ -700,6 +697,9 @@
   <si>
     <t>UPANEMA - VARA ÚNICA</t>
   </si>
+  <si>
+    <t>NATAL - 1ª VARA REGIONAL DE EXECUÇÃO PENAL</t>
+  </si>
 </sst>
 </file>
 
@@ -42097,7 +42097,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78A0B8ED-4951-4ABA-BF26-3370CEFE35BA}">
   <dimension ref="A1:D217"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A105" sqref="A105"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -43708,14 +43710,12 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B101" s="5">
-        <f>VLOOKUP(A101,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
         <v>100</v>
       </c>
       <c r="C101" s="5">
-        <f>VLOOKUP(A101,'[1]jan-19 31-mai-2020'!$B:$D,3,0)</f>
         <v>16</v>
       </c>
       <c r="D101" s="6">
@@ -43724,14 +43724,12 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B102" s="5">
-        <f>VLOOKUP(A102,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
         <v>101</v>
       </c>
       <c r="C102" s="5">
-        <f>VLOOKUP(A102,'[1]jan-19 31-mai-2020'!$B:$D,3,0)</f>
         <v>14</v>
       </c>
       <c r="D102" s="6">
@@ -43740,14 +43738,12 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B103" s="5">
-        <f>VLOOKUP(A103,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
         <v>102</v>
       </c>
       <c r="C103" s="5">
-        <f>VLOOKUP(A103,'[1]jan-19 31-mai-2020'!$B:$D,3,0)</f>
         <v>15</v>
       </c>
       <c r="D103" s="6">
@@ -43756,14 +43752,12 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B104" s="5">
-        <f>VLOOKUP(A104,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
         <v>103</v>
       </c>
       <c r="C104" s="5">
-        <f>VLOOKUP(A104,'[1]jan-19 31-mai-2020'!$B:$D,3,0)</f>
         <v>17</v>
       </c>
       <c r="D104" s="6">
@@ -43772,14 +43766,12 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>107</v>
+        <v>219</v>
       </c>
       <c r="B105" s="5">
-        <f>VLOOKUP(A105,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
         <v>104</v>
       </c>
       <c r="C105" s="5">
-        <f>VLOOKUP(A105,'[1]jan-19 31-mai-2020'!$B:$D,3,0)</f>
         <v>18</v>
       </c>
       <c r="D105" s="6">
@@ -43788,7 +43780,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B106" s="5">
         <f>VLOOKUP(A106,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -43804,7 +43796,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B107" s="5">
         <f>VLOOKUP(A107,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -43820,7 +43812,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B108" s="5">
         <f>VLOOKUP(A108,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -43836,7 +43828,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B109" s="5">
         <f>VLOOKUP(A109,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -43852,7 +43844,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B110" s="5">
         <f>VLOOKUP(A110,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -43868,7 +43860,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B111" s="5">
         <f>VLOOKUP(A111,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -43884,7 +43876,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B112" s="5">
         <f>VLOOKUP(A112,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -43900,7 +43892,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B113" s="5">
         <f>VLOOKUP(A113,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -43916,7 +43908,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B114" s="5">
         <f>VLOOKUP(A114,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -43932,7 +43924,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B115" s="5">
         <f>VLOOKUP(A115,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -43948,7 +43940,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B116" s="5">
         <f>VLOOKUP(A116,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -43964,7 +43956,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B117" s="5">
         <f>VLOOKUP(A117,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -43980,7 +43972,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B118" s="5">
         <f>VLOOKUP(A118,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -43996,7 +43988,7 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B119" s="5">
         <f>VLOOKUP(A119,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44012,7 +44004,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B120" s="5">
         <f>VLOOKUP(A120,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44028,7 +44020,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B121" s="5">
         <f>VLOOKUP(A121,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44044,7 +44036,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B122" s="5">
         <f>VLOOKUP(A122,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44060,7 +44052,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B123" s="5">
         <f>VLOOKUP(A123,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44076,7 +44068,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B124" s="5">
         <f>VLOOKUP(A124,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44092,7 +44084,7 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B125" s="5">
         <f>VLOOKUP(A125,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44108,7 +44100,7 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B126" s="5">
         <f>VLOOKUP(A126,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44124,7 +44116,7 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B127" s="5">
         <f>VLOOKUP(A127,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44140,7 +44132,7 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B128" s="5">
         <f>VLOOKUP(A128,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44156,7 +44148,7 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B129" s="5">
         <f>VLOOKUP(A129,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44172,7 +44164,7 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B130" s="5">
         <f>VLOOKUP(A130,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44188,7 +44180,7 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B131" s="5">
         <f>VLOOKUP(A131,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44204,7 +44196,7 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B132" s="5">
         <f>VLOOKUP(A132,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44220,7 +44212,7 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B133" s="5">
         <f>VLOOKUP(A133,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44236,7 +44228,7 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B134" s="5">
         <f>VLOOKUP(A134,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44252,7 +44244,7 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B135" s="5">
         <f>VLOOKUP(A135,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44268,7 +44260,7 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B136" s="5">
         <f>VLOOKUP(A136,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44284,7 +44276,7 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B137" s="5">
         <f>VLOOKUP(A137,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44300,7 +44292,7 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B138" s="5">
         <f>VLOOKUP(A138,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44316,7 +44308,7 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B139" s="5">
         <f>VLOOKUP(A139,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44332,7 +44324,7 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B140" s="5">
         <f>VLOOKUP(A140,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44348,7 +44340,7 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B141" s="5">
         <f>VLOOKUP(A141,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44364,7 +44356,7 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B142" s="5">
         <f>VLOOKUP(A142,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44380,7 +44372,7 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B143" s="5">
         <f>VLOOKUP(A143,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44396,7 +44388,7 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B144" s="5">
         <f>VLOOKUP(A144,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44412,7 +44404,7 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B145" s="5">
         <f>VLOOKUP(A145,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44428,7 +44420,7 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B146" s="5">
         <f>VLOOKUP(A146,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44444,7 +44436,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B147" s="5">
         <f>VLOOKUP(A147,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44460,7 +44452,7 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B148" s="5">
         <f>VLOOKUP(A148,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44476,7 +44468,7 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B149" s="5">
         <f>VLOOKUP(A149,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44492,7 +44484,7 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B150" s="5">
         <f>VLOOKUP(A150,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44508,7 +44500,7 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B151" s="5">
         <f>VLOOKUP(A151,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44524,7 +44516,7 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B152" s="5">
         <f>VLOOKUP(A152,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44540,7 +44532,7 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B153" s="5">
         <f>VLOOKUP(A153,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44556,7 +44548,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B154" s="5">
         <f>VLOOKUP(A154,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44572,7 +44564,7 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B155" s="5">
         <f>VLOOKUP(A155,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44588,7 +44580,7 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B156" s="5">
         <f>VLOOKUP(A156,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44604,7 +44596,7 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B157" s="5">
         <f>VLOOKUP(A157,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44620,7 +44612,7 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B158" s="5">
         <f>VLOOKUP(A158,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44636,7 +44628,7 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B159" s="5">
         <f>VLOOKUP(A159,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44652,7 +44644,7 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B160" s="5">
         <f>VLOOKUP(A160,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44668,7 +44660,7 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B161" s="5">
         <f>VLOOKUP(A161,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44684,7 +44676,7 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B162" s="5">
         <f>VLOOKUP(A162,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44700,7 +44692,7 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B163" s="5">
         <f>VLOOKUP(A163,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44716,7 +44708,7 @@
     </row>
     <row r="164" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B164" s="5">
         <f>VLOOKUP(A164,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44732,7 +44724,7 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B165" s="5">
         <f>VLOOKUP(A165,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44748,7 +44740,7 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B166" s="5">
         <f>VLOOKUP(A166,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44764,7 +44756,7 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B167" s="5">
         <f>VLOOKUP(A167,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44780,7 +44772,7 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B168" s="5">
         <f>VLOOKUP(A168,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44796,7 +44788,7 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B169" s="5">
         <f>VLOOKUP(A169,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44812,7 +44804,7 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B170" s="5">
         <f>VLOOKUP(A170,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44828,7 +44820,7 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B171" s="5">
         <f>VLOOKUP(A171,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44844,7 +44836,7 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B172" s="5">
         <f>VLOOKUP(A172,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44860,7 +44852,7 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B173" s="5">
         <f>VLOOKUP(A173,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44876,7 +44868,7 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B174" s="5">
         <f>VLOOKUP(A174,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44892,7 +44884,7 @@
     </row>
     <row r="175" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A175" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B175" s="5">
         <f>VLOOKUP(A175,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44908,7 +44900,7 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B176" s="5">
         <f>VLOOKUP(A176,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44924,7 +44916,7 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B177" s="5">
         <f>VLOOKUP(A177,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44940,7 +44932,7 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B178" s="5">
         <f>VLOOKUP(A178,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44956,7 +44948,7 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B179" s="5">
         <f>VLOOKUP(A179,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44972,7 +44964,7 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B180" s="5">
         <f>VLOOKUP(A180,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -44988,7 +44980,7 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B181" s="5">
         <f>VLOOKUP(A181,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45004,7 +44996,7 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B182" s="5">
         <f>VLOOKUP(A182,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45020,7 +45012,7 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B183" s="5">
         <f>VLOOKUP(A183,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45036,7 +45028,7 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B184" s="5">
         <f>VLOOKUP(A184,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45052,7 +45044,7 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B185" s="5">
         <f>VLOOKUP(A185,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45068,7 +45060,7 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B186" s="5">
         <f>VLOOKUP(A186,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45084,7 +45076,7 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B187" s="5">
         <f>VLOOKUP(A187,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45100,7 +45092,7 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B188" s="5">
         <f>VLOOKUP(A188,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45116,7 +45108,7 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B189" s="5">
         <f>VLOOKUP(A189,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45132,7 +45124,7 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B190" s="5">
         <f>VLOOKUP(A190,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45148,7 +45140,7 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B191" s="5">
         <f>VLOOKUP(A191,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45164,7 +45156,7 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B192" s="5">
         <f>VLOOKUP(A192,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45180,7 +45172,7 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B193" s="5">
         <f>VLOOKUP(A193,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45196,7 +45188,7 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B194" s="5">
         <f>VLOOKUP(A194,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45212,7 +45204,7 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B195" s="5">
         <f>VLOOKUP(A195,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45228,7 +45220,7 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B196" s="5">
         <f>VLOOKUP(A196,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45244,7 +45236,7 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B197" s="5">
         <f>VLOOKUP(A197,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45260,7 +45252,7 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B198" s="5">
         <f>VLOOKUP(A198,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45276,7 +45268,7 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B199" s="5">
         <f>VLOOKUP(A199,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45292,7 +45284,7 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B200" s="5">
         <f>VLOOKUP(A200,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45308,7 +45300,7 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B201" s="5">
         <f>VLOOKUP(A201,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45324,7 +45316,7 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B202" s="5">
         <f>VLOOKUP(A202,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45340,7 +45332,7 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B203" s="5">
         <f>VLOOKUP(A203,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45356,7 +45348,7 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B204" s="5">
         <f>VLOOKUP(A204,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45372,7 +45364,7 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B205" s="5">
         <f>VLOOKUP(A205,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45388,7 +45380,7 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B206" s="5">
         <f>VLOOKUP(A206,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45404,7 +45396,7 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B207" s="5">
         <f>VLOOKUP(A207,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45420,7 +45412,7 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B208" s="5">
         <f>VLOOKUP(A208,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45436,7 +45428,7 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B209" s="5">
         <f>VLOOKUP(A209,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45452,7 +45444,7 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B210" s="5">
         <f>VLOOKUP(A210,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45468,7 +45460,7 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B211" s="5">
         <f>VLOOKUP(A211,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45484,7 +45476,7 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B212" s="5">
         <f>VLOOKUP(A212,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45500,7 +45492,7 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B213" s="5">
         <f>VLOOKUP(A213,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45516,7 +45508,7 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B214" s="5">
         <f>VLOOKUP(A214,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45532,7 +45524,7 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B215" s="5">
         <f>VLOOKUP(A215,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45548,7 +45540,7 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B216" s="5">
         <f>VLOOKUP(A216,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>
@@ -45564,7 +45556,7 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B217" s="5">
         <f>VLOOKUP(A217,'[1]jan-19 31-mai-2020'!$B:$D,2,0)</f>

</xml_diff>